<commit_message>
new spreadsheet and poster
</commit_message>
<xml_diff>
--- a/Edu. Research/ProgrammingingeophysicsPost.xlsx
+++ b/Edu. Research/ProgrammingingeophysicsPost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julien-Pooya/Downloads/Downloads Safari/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julien-Pooya/Documents/GitHub/GEOF_UiB/Edu. Research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA17C55-4750-274E-9ED4-5390A2B933FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4F9635-C18D-6B4C-8187-E8702BF93E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5000" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProgrammingingeophysicsII" sheetId="1" r:id="rId1"/>
@@ -239,6 +239,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -599,10 +600,23 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:O8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="58.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="57" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>